<commit_message>
Small Error in Every Mod file
</commit_message>
<xml_diff>
--- a/BaseCase/BasecaseComparison.xlsx
+++ b/BaseCase/BasecaseComparison.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jannik/Documents/Master/EPFL/Github/ModAndOptOfEnergySystems/BaseCase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Vincent/ModAndOptOfEnergySystem/BaseCase/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1180" windowWidth="27880" windowHeight="15220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,6 +66,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,9 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -162,7 +164,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Sheet1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -200,19 +202,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2.0380322E7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6724613E7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.2134257E7</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -222,7 +215,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -260,19 +253,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:f>Sheet1!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7.91403758748286E6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.77907E6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.874772E6</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -282,7 +266,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Sheet1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -320,19 +304,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$D$4</c:f>
+              <c:f>Sheet1!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7.407769E6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.545127E6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.464427E6</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -342,7 +317,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Sheet1!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -380,19 +355,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$D$5</c:f>
+              <c:f>Sheet1!$B$7:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>506268.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>233942.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>410345.0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -407,11 +373,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-68990896"/>
-        <c:axId val="-68998704"/>
+        <c:axId val="895823040"/>
+        <c:axId val="909816032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-68990896"/>
+        <c:axId val="895823040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -454,7 +420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-68998704"/>
+        <c:crossAx val="909816032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -462,7 +428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-68998704"/>
+        <c:axId val="909816032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,7 +478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-68990896"/>
+        <c:crossAx val="895823040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1142,14 +1108,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1434,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,60 +1420,45 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>20380322</v>
-      </c>
-      <c r="C2">
-        <v>16724613</v>
-      </c>
-      <c r="D2" s="1">
-        <v>12134257</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>7914037.5874828603</v>
-      </c>
-      <c r="C3" s="1">
-        <v>7779070</v>
-      </c>
-      <c r="D3" s="1">
-        <v>7874772</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>7407769</v>
-      </c>
-      <c r="C4" s="1">
-        <v>7545127</v>
-      </c>
-      <c r="D4" s="1">
-        <v>7464427</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
-        <v>506268</v>
-      </c>
-      <c r="C5" s="1">
-        <v>233942</v>
-      </c>
-      <c r="D5" s="1">
-        <v>410345</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>